<commit_message>
updates to Animal model forthcoming
</commit_message>
<xml_diff>
--- a/SHACL/CJ16050Constraints/TestCases.xlsx
+++ b/SHACL/CJ16050Constraints/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\SENDConform\SHACL\CJ16050Constraints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089F3B58-C3FE-4FBA-81F9-F770E7E69778}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48400B64-3F5A-4BD8-A736-81D6E495185C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5770" activeTab="2" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5770" activeTab="1" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="134">
   <si>
     <t>SD1002</t>
   </si>
@@ -566,6 +566,18 @@
     <t>Age missing when not required (armcd=NOTASSGN)</t>
   </si>
   <si>
+    <t>Data Pass/Fail</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> age missing when required:   age = NA AND (NOT  (ARMCD=SCRNFAIL || ARMCD=NOTASSGN ))</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">missing </t>
     </r>
@@ -599,20 +611,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>armd=NOTASSGN</t>
-    </r>
-  </si>
-  <si>
-    <t>Data Pass/Fail</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> age missing when equired:   age = NA AND (NOT  (ARMCD=SCRNFAIL || ARMCD=NOTASSGN ))</t>
+      <t>armcd=NOTASSGN</t>
+    </r>
+  </si>
+  <si>
+    <t>Link our data to teh SEND ontology</t>
   </si>
 </sst>
 </file>
@@ -815,7 +818,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -911,6 +914,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1328,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B000AF4-3217-4B69-866D-C06BDBC2A333}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1532,6 +1538,9 @@
       <c r="E11" s="36" t="s">
         <v>18</v>
       </c>
+      <c r="F11" s="37" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="65" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -1715,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F07C322-D3AE-4F2B-B5AA-83448FAE9597}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1742,7 +1751,7 @@
         <v>120</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>98</v>
@@ -1765,7 +1774,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2" s="22" t="s">
         <v>107</v>
@@ -1786,7 +1795,7 @@
         <v>99</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>106</v>
@@ -1809,7 +1818,7 @@
         <v>101</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F4" s="28" t="s">
         <v>106</v>
@@ -1830,7 +1839,7 @@
         <v>100</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>105</v>
@@ -1851,7 +1860,7 @@
         <v>111</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="21" t="s">
@@ -1872,7 +1881,7 @@
         <v>123</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="21"/>
@@ -1891,7 +1900,7 @@
         <v>124</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F8" s="28" t="s">
         <v>106</v>
@@ -1912,7 +1921,7 @@
         <v>101</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F9" s="28" t="s">
         <v>106</v>
@@ -1942,13 +1951,13 @@
         <v>112</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>126</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="21"/>
@@ -1962,10 +1971,10 @@
         <v>127</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="21"/>

</xml_diff>

<commit_message>
reworked documentation for the first constraint.
</commit_message>
<xml_diff>
--- a/SHACL/CJ16050Constraints/TestCases.xlsx
+++ b/SHACL/CJ16050Constraints/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\SENDConform\SHACL\CJ16050Constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA6CC6B-2F29-4E8E-8300-955031DC3828}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D41461-0C23-4D21-80C3-2917AC01D1A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5770" activeTab="2" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="145">
   <si>
     <t>SD1002</t>
   </si>
@@ -452,9 +452,6 @@
     <t>Start Date must be on or before End Date</t>
   </si>
   <si>
-    <t>:DateShape</t>
-  </si>
-  <si>
     <t>:RefIntervalShape</t>
   </si>
   <si>
@@ -548,9 +545,6 @@
     <t>Age missing when not required (armcd=NOTASSGN)</t>
   </si>
   <si>
-    <t>Data Pass/Fail</t>
-  </si>
-  <si>
     <t>FAIL</t>
   </si>
   <si>
@@ -606,10 +600,6 @@
     <t>99T6,99T7</t>
   </si>
   <si>
-    <t>Rule
-Component</t>
-  </si>
-  <si>
     <t>Start Date and End Date in date (xsd:date) format</t>
   </si>
   <si>
@@ -665,11 +655,38 @@
   <si>
     <t>Missing rfendtc (start with no end)</t>
   </si>
+  <si>
+    <t>99T10</t>
+  </si>
+  <si>
+    <t>rfstdtc as xsd:string  "6-DEC-2016"</t>
+  </si>
+  <si>
+    <t>:DateFmtShape</t>
+  </si>
+  <si>
+    <t>Rule
+Comp.</t>
+  </si>
+  <si>
+    <t>Eval
+date</t>
+  </si>
+  <si>
+    <t>Expected Pass/Fail</t>
+  </si>
+  <si>
+    <t>Test
+Status</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -872,7 +889,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -921,7 +938,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1000,18 +1016,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="1" xr:uid="{B3B9F93B-6BDF-408F-A1F2-4D90ACF3B2E0}"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1541,7 +1595,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>61</v>
@@ -1558,7 +1612,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>29</v>
@@ -1601,17 +1655,17 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="32" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1633,21 +1687,21 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35" t="s">
+      <c r="B11" s="33"/>
+      <c r="C11" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="37" t="s">
-        <v>127</v>
+      <c r="F11" s="36" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -1830,501 +1884,617 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F07C322-D3AE-4F2B-B5AA-83448FAE9597}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.90625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.36328125" style="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.36328125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" style="17" customWidth="1"/>
     <col min="5" max="5" width="42.36328125" style="17" customWidth="1"/>
     <col min="6" max="6" width="9.1796875" style="17" customWidth="1"/>
     <col min="7" max="7" width="20.36328125" customWidth="1"/>
-    <col min="8" max="8" width="34.26953125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="6.54296875" style="39" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.26953125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="39" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>100</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="38">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+      <c r="I2" s="51">
+        <v>43678</v>
+      </c>
+      <c r="J2" s="20"/>
+    </row>
+    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="21"/>
+      <c r="B3" s="38">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" s="51">
+        <v>43678</v>
+      </c>
+      <c r="J3" s="20"/>
+    </row>
+    <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39">
-        <v>1</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="B4" s="38">
+        <v>2</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="F4" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="21" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="45">
+        <v>2</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="27"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="20"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="45">
+        <v>2</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
+    </row>
+    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="45">
+        <v>2</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F7" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="46"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="38">
+        <v>3</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="50"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="20"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="21"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="20"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="21"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="20"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="21"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="20"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="21"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="21"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="20"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="21"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="20"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="21"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="20"/>
+    </row>
+    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" s="21"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="40"/>
+      <c r="C17" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G17" s="21"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="A18" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="41"/>
+      <c r="C18" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="50"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="20"/>
+    </row>
+    <row r="19" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="A19" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" s="50"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="20"/>
+    </row>
+    <row r="20" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="42"/>
+      <c r="C20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="43"/>
+      <c r="C21" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="G2" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="21"/>
-    </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="39">
-        <v>2</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="46">
-        <v>2</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="D4" s="22" t="s">
+      <c r="D21" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="20"/>
+    </row>
+    <row r="22" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="21"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="21"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="46">
-        <v>2</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>138</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="46">
-        <v>2</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="E6" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="G6" s="48"/>
-      <c r="H6" s="21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="39">
-        <v>3</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="G7" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="22"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="21"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="21"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="22"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="22"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="22"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="22"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="21"/>
-    </row>
-    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="17" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A17" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="H17" s="21"/>
-    </row>
-    <row r="18" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A18" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="H18" s="21"/>
-    </row>
-    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="21"/>
-    </row>
-    <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="22"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="F21" s="21" t="s">
+      <c r="E22" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="22"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="21"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="22"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="21"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="22"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="21"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="22"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="21"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="22"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="21"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="22"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="21"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="22"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="21"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="22"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="21"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="22"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="21"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="22"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="21"/>
+      <c r="F22" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="20"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="21"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="20"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="21"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="20"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="21"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="20"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="21"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="20"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="21"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="20"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="21"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="20"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="21"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="20"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="21"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="20"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="21"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="20"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="21"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="20"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F4 F7:F30">
+  <conditionalFormatting sqref="F8:F31 F2:F5">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2332,7 +2502,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31">
+  <conditionalFormatting sqref="F6">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2340,7 +2510,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
+  <conditionalFormatting sqref="H2">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2348,7 +2518,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
+  <conditionalFormatting sqref="H3:H32">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>

</xml_diff>

<commit_message>
SD1002 SHACL - all rules working.
</commit_message>
<xml_diff>
--- a/SHACL/CJ16050Constraints/TestCases.xlsx
+++ b/SHACL/CJ16050Constraints/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\SENDConform\SHACL\CJ16050Constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D41461-0C23-4D21-80C3-2917AC01D1A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC18F9B-7190-410B-AEC3-772A5C7C5C7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5770" activeTab="2" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="149">
   <si>
     <t>SD1002</t>
   </si>
@@ -455,9 +455,6 @@
     <t>:RefIntervalShape</t>
   </si>
   <si>
-    <t>:SD1002RuleShape</t>
-  </si>
-  <si>
     <t>Unique USUBJID</t>
   </si>
   <si>
@@ -609,60 +606,16 @@
     <t>One RFSTDTC/RFENDTC per AnimalSubject</t>
   </si>
   <si>
-    <r>
-      <t>More than one RFSTDTC and RDFENDTC for a single subject  :</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> TWO reference intervals</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">missing rfstdtc AND missing rfendtc = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NO reference interval</t>
-    </r>
-  </si>
-  <si>
-    <t>no reference interval created</t>
-  </si>
-  <si>
     <t>99T8</t>
   </si>
   <si>
     <t>99T9</t>
   </si>
   <si>
-    <t>Missing stdtc  (end with no start)</t>
-  </si>
-  <si>
-    <t>Missing rfendtc (start with no end)</t>
-  </si>
-  <si>
     <t>99T10</t>
   </si>
   <si>
     <t>rfstdtc as xsd:string  "6-DEC-2016"</t>
-  </si>
-  <si>
-    <t>:DateFmtShape</t>
   </si>
   <si>
     <t>Rule
@@ -678,6 +631,41 @@
   <si>
     <t>Test
 Status</t>
+  </si>
+  <si>
+    <t>No Interval IRI (and not start and end dates)</t>
+  </si>
+  <si>
+    <t>DateFmtShape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it is possible for an interval to be present but lacking dates. </t>
+  </si>
+  <si>
+    <t>SD1002RuleShape</t>
+  </si>
+  <si>
+    <t>RefIntervalDateShape</t>
+  </si>
+  <si>
+    <t>Interval has missing rfendtc (start with no end)</t>
+  </si>
+  <si>
+    <t>Interval has missing stdtc  (end with no start)</t>
+  </si>
+  <si>
+    <t>Interval  has missing rfstdtc and rfendtc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interval with &gt;1 rfstdtc and &gt;1 rfendtc </t>
+  </si>
+  <si>
+    <t>:AnimalOneRefIntervalShape</t>
+  </si>
+  <si>
+    <t>99T11
+99T2
+99T</t>
   </si>
 </sst>
 </file>
@@ -685,9 +673,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -779,6 +767,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -889,7 +884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1016,9 +1011,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1029,15 +1021,112 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="1" xr:uid="{B3B9F93B-6BDF-408F-A1F2-4D90ACF3B2E0}"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1595,7 +1684,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>61</v>
@@ -1612,7 +1701,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>29</v>
@@ -1701,7 +1790,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -1884,15 +1973,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F07C322-D3AE-4F2B-B5AA-83448FAE9597}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="6.36328125" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" style="39" customWidth="1"/>
     <col min="3" max="3" width="38.36328125" style="17" customWidth="1"/>
     <col min="4" max="4" width="11.90625" style="17" customWidth="1"/>
     <col min="5" max="5" width="42.36328125" style="17" customWidth="1"/>
@@ -1908,7 +1997,7 @@
         <v>74</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>100</v>
@@ -1917,22 +2006,22 @@
         <v>96</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="I1" s="49" t="s">
-        <v>142</v>
+      <c r="H1" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>135</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1943,24 +2032,24 @@
         <v>1</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>129</v>
-      </c>
       <c r="F2" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="I2" s="51">
+      <c r="I2" s="50">
         <v>43678</v>
       </c>
       <c r="J2" s="20"/>
@@ -1971,200 +2060,195 @@
         <v>1</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E3" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="H3" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="G3" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="I3" s="51">
+      <c r="I3" s="50">
         <v>43678</v>
       </c>
       <c r="J3" s="20"/>
     </row>
-    <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="38">
-        <v>2</v>
-      </c>
+      <c r="B4" s="45"/>
       <c r="C4" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>131</v>
+        <v>107</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>143</v>
       </c>
       <c r="F4" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="20" t="s">
-        <v>110</v>
-      </c>
+      <c r="I4" s="50">
+        <v>43681</v>
+      </c>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="45">
-        <v>2</v>
-      </c>
+      <c r="B5" s="45"/>
       <c r="C5" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>137</v>
+        <v>129</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="F5" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="20"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I5" s="50">
+        <v>43681</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="45">
-        <v>2</v>
-      </c>
+      <c r="B6" s="53"/>
       <c r="C6" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>136</v>
+      <c r="E6" s="44" t="s">
+        <v>145</v>
       </c>
       <c r="F6" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="51"/>
+      <c r="I6" s="50">
+        <v>43681</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="45">
-        <v>2</v>
-      </c>
+      <c r="B7" s="38"/>
       <c r="C7" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>132</v>
+        <v>129</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="F7" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="H7" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="46"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="51"/>
+      <c r="I7" s="50">
+        <v>43681</v>
+      </c>
       <c r="J7" s="20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="38">
-        <v>3</v>
-      </c>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="39">
+        <v>4</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="H8" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="I8" s="50">
+        <v>43681</v>
+      </c>
+      <c r="J8" s="20"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="20" t="s">
+      <c r="D12" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="50"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="21"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="51"/>
+      <c r="F12" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="H12" s="49"/>
+      <c r="I12" s="50"/>
       <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -2174,9 +2258,9 @@
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="51"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
       <c r="J13" s="20"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -2186,9 +2270,9 @@
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="51"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="50"/>
       <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -2198,211 +2282,211 @@
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="51"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="50"/>
       <c r="J15" s="20"/>
     </row>
-    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="21"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="21"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="21"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="20"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="21"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="20"/>
+    </row>
+    <row r="20" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="20" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="21"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="40"/>
+      <c r="C21" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="E16" s="20" t="s">
+      <c r="E21" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="20"/>
+    </row>
+    <row r="22" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="A22" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="C22" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="H22" s="49"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="20"/>
+    </row>
+    <row r="23" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="A23" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="41"/>
+      <c r="C23" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="49"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="20"/>
+    </row>
+    <row r="24" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="42"/>
+      <c r="C24" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="28"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="43"/>
+      <c r="C25" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="1:10" ht="26" x14ac:dyDescent="0.35">
-      <c r="A18" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="H18" s="50"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="1:10" ht="26" x14ac:dyDescent="0.35">
-      <c r="A19" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G19" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="H19" s="50"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="20"/>
-    </row>
-    <row r="20" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="30" t="s">
+      <c r="E25" s="20" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G21" s="21"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="21"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="20" t="s">
+      <c r="F25" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="20"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="21"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="20"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="21"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="20"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="21"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="51"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="21"/>
       <c r="B26" s="38"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
+      <c r="C26" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>121</v>
+      </c>
       <c r="G26" s="21"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="51"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="50"/>
       <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -2413,8 +2497,8 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="21"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="51"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="50"/>
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -2425,8 +2509,8 @@
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="21"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="51"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="50"/>
       <c r="J28" s="20"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -2437,8 +2521,8 @@
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="21"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="51"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="50"/>
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -2449,8 +2533,8 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="51"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -2461,8 +2545,8 @@
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
       <c r="G31" s="21"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="51"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="50"/>
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -2473,36 +2557,124 @@
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
       <c r="G32" s="21"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="51"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="50"/>
       <c r="J32" s="20"/>
     </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="21"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="20"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="21"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="20"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" s="21"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="20"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="21"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="20"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F8:F31 F2:F5">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+  <conditionalFormatting sqref="F2:F4 G4 H12:H36 H3:H6 F12:F35 F7:F8">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+  <conditionalFormatting sqref="F36">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2510,7 +2682,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="G8">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2518,7 +2690,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H32">
+  <conditionalFormatting sqref="H8">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>

</xml_diff>

<commit_message>
updates to test case list
</commit_message>
<xml_diff>
--- a/SHACL/CJ16050Constraints/TestCases.xlsx
+++ b/SHACL/CJ16050Constraints/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\SENDConform\SHACL\CJ16050Constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC18F9B-7190-410B-AEC3-772A5C7C5C7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F18865-B2CF-46CE-A55C-85BE60BDF254}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5770" activeTab="2" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5775" activeTab="2" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="152">
   <si>
     <t>SD1002</t>
   </si>
@@ -449,9 +449,6 @@
     <t>Rule Component</t>
   </si>
   <si>
-    <t>Start Date must be on or before End Date</t>
-  </si>
-  <si>
     <t>:RefIntervalShape</t>
   </si>
   <si>
@@ -597,9 +594,6 @@
     <t>99T6,99T7</t>
   </si>
   <si>
-    <t>Start Date and End Date in date (xsd:date) format</t>
-  </si>
-  <si>
     <t>rfendtc as xsd:string  "7-Dec-2016"</t>
   </si>
   <si>
@@ -616,10 +610,6 @@
   </si>
   <si>
     <t>rfstdtc as xsd:string  "6-DEC-2016"</t>
-  </si>
-  <si>
-    <t>Rule
-Comp.</t>
   </si>
   <si>
     <t>Eval
@@ -658,14 +648,33 @@
   </si>
   <si>
     <t xml:space="preserve">Interval with &gt;1 rfstdtc and &gt;1 rfendtc </t>
-  </si>
-  <si>
-    <t>:AnimalOneRefIntervalShape</t>
   </si>
   <si>
     <t>99T11
 99T2
 99T</t>
+  </si>
+  <si>
+    <t>Rule
+Component</t>
+  </si>
+  <si>
+    <t> Reference Start Date and End Date in xsd:date format</t>
+  </si>
+  <si>
+    <t>A Reference Interval has one Start Date and one End Date</t>
+  </si>
+  <si>
+    <t>A Subject has one Reference Interval</t>
+  </si>
+  <si>
+    <t>The SD1002 Rule itself: Start Date on or before End Date</t>
+  </si>
+  <si>
+    <t>SubjectOneRefIntervalShape</t>
+  </si>
+  <si>
+    <t>Rules under development</t>
   </si>
 </sst>
 </file>
@@ -772,8 +781,10 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1024,9 +1035,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1037,6 +1045,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1533,44 +1542,44 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -1589,17 +1598,17 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.1796875" customWidth="1"/>
-    <col min="4" max="4" width="36.54296875" customWidth="1"/>
-    <col min="5" max="5" width="35.54296875" customWidth="1"/>
-    <col min="6" max="6" width="29.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>74</v>
       </c>
@@ -1619,7 +1628,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="91" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="102" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>43</v>
       </c>
@@ -1639,7 +1648,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="104" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
@@ -1659,7 +1668,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="91" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="102" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -1679,12 +1688,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>61</v>
@@ -1696,12 +1705,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>29</v>
@@ -1713,7 +1722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="65" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="65" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -1743,7 +1752,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>56</v>
       </c>
@@ -1758,7 +1767,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1775,7 +1784,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>15</v>
       </c>
@@ -1790,10 +1799,10 @@
         <v>18</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="65" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1808,7 +1817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="52" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1838,7 +1847,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1853,7 +1862,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>52</v>
       </c>
@@ -1868,7 +1877,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1883,7 +1892,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1898,7 +1907,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>71</v>
       </c>
@@ -1913,7 +1922,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>67</v>
       </c>
@@ -1928,7 +1937,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
@@ -1943,7 +1952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -1973,31 +1982,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F07C322-D3AE-4F2B-B5AA-83448FAE9597}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.81640625" style="39" customWidth="1"/>
-    <col min="3" max="3" width="38.36328125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="42.36328125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="17" customWidth="1"/>
-    <col min="7" max="7" width="20.36328125" customWidth="1"/>
-    <col min="8" max="8" width="6.54296875" style="39" customWidth="1"/>
-    <col min="9" max="9" width="10.08984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.26953125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="39" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="39" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.28515625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>100</v>
@@ -2006,25 +2015,25 @@
         <v>96</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>98</v>
       </c>
       <c r="H1" s="48" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I1" s="48" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -2032,464 +2041,483 @@
         <v>1</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F2" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" s="49" t="s">
         <v>120</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="H2" s="49" t="s">
-        <v>121</v>
       </c>
       <c r="I2" s="50">
         <v>43678</v>
       </c>
       <c r="J2" s="20"/>
     </row>
-    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="38">
         <v>1</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F3" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="49" t="s">
         <v>120</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="H3" s="49" t="s">
-        <v>121</v>
       </c>
       <c r="I3" s="50">
         <v>43678</v>
       </c>
       <c r="J3" s="20"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="45">
+        <v>3</v>
+      </c>
       <c r="C4" s="20" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F4" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="49" t="s">
         <v>120</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="H4" s="49" t="s">
-        <v>121</v>
       </c>
       <c r="I4" s="50">
         <v>43681</v>
       </c>
       <c r="J4" s="20"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="45"/>
+      <c r="B5" s="45">
+        <v>3</v>
+      </c>
       <c r="C5" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="47" t="s">
-        <v>131</v>
-      </c>
       <c r="E5" s="17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F5" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="49" t="s">
         <v>120</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="H5" s="49" t="s">
-        <v>121</v>
       </c>
       <c r="I5" s="50">
         <v>43681</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="52">
+        <v>3</v>
+      </c>
       <c r="C6" s="20" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F6" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="H6" s="49" t="s">
         <v>120</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>121</v>
       </c>
       <c r="I6" s="50">
         <v>43681</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="38">
+        <v>3</v>
+      </c>
       <c r="C7" s="20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F7" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="49" t="s">
         <v>120</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="H7" s="49" t="s">
-        <v>121</v>
       </c>
       <c r="I7" s="50">
         <v>43681</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="52" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="51" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="39">
-        <v>4</v>
-      </c>
-      <c r="C8" s="54" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="E8" s="51" t="s">
-        <v>138</v>
+      <c r="D8" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>135</v>
       </c>
       <c r="F8" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="49" t="s">
         <v>120</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="H8" s="49" t="s">
-        <v>121</v>
       </c>
       <c r="I8" s="50">
         <v>43681</v>
       </c>
       <c r="J8" s="20"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" s="20" t="s">
+      <c r="B9" s="38">
+        <v>4</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="I9" s="50">
+        <v>43681</v>
+      </c>
+      <c r="J9" s="20"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="55" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="G12" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="H12" s="49"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="21"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="46"/>
+      <c r="F13" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="21"/>
       <c r="H13" s="49"/>
       <c r="I13" s="50"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="46"/>
+      <c r="J13" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="40"/>
+      <c r="C14" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="21"/>
       <c r="H14" s="49"/>
       <c r="I14" s="50"/>
       <c r="J14" s="20"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="46"/>
+    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="41"/>
+      <c r="C15" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>101</v>
+      </c>
       <c r="H15" s="49"/>
       <c r="I15" s="50"/>
       <c r="J15" s="20"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="46"/>
+    <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="41"/>
+      <c r="C16" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>101</v>
+      </c>
       <c r="H16" s="49"/>
       <c r="I16" s="50"/>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="42"/>
+      <c r="C17" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="30"/>
       <c r="F17" s="20"/>
-      <c r="G17" s="46"/>
+      <c r="G17" s="31"/>
       <c r="H17" s="49"/>
       <c r="I17" s="50"/>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="21"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="46"/>
+      <c r="J17" s="30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="21"/>
       <c r="H18" s="49"/>
       <c r="I18" s="50"/>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="38"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="46"/>
+      <c r="C19" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="21"/>
       <c r="H19" s="49"/>
       <c r="I19" s="50"/>
       <c r="J19" s="20"/>
     </row>
-    <row r="20" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="21" t="s">
-        <v>60</v>
-      </c>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
       <c r="B20" s="38"/>
-      <c r="C20" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>120</v>
-      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
       <c r="G20" s="21"/>
       <c r="H20" s="49"/>
       <c r="I20" s="50"/>
-      <c r="J20" s="20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>120</v>
-      </c>
+      <c r="J20" s="20"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
       <c r="G21" s="21"/>
       <c r="H21" s="49"/>
       <c r="I21" s="50"/>
       <c r="J21" s="20"/>
     </row>
-    <row r="22" spans="1:10" ht="26" x14ac:dyDescent="0.35">
-      <c r="A22" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="G22" s="27" t="s">
-        <v>102</v>
-      </c>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="21"/>
       <c r="H22" s="49"/>
       <c r="I22" s="50"/>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" spans="1:10" ht="26" x14ac:dyDescent="0.35">
-      <c r="A23" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="G23" s="27" t="s">
-        <v>102</v>
-      </c>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
       <c r="H23" s="49"/>
       <c r="I23" s="50"/>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="30"/>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="20"/>
-      <c r="G24" s="31"/>
+      <c r="G24" s="21"/>
       <c r="H24" s="49"/>
       <c r="I24" s="50"/>
-      <c r="J24" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>120</v>
-      </c>
+      <c r="J24" s="20"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="21"/>
       <c r="H25" s="49"/>
       <c r="I25" s="50"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="38"/>
-      <c r="C26" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>121</v>
-      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
       <c r="G26" s="21"/>
       <c r="H26" s="49"/>
       <c r="I26" s="50"/>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="38"/>
       <c r="C27" s="20"/>
@@ -2501,7 +2529,7 @@
       <c r="I27" s="50"/>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="38"/>
       <c r="C28" s="20"/>
@@ -2513,7 +2541,7 @@
       <c r="I28" s="50"/>
       <c r="J28" s="20"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
       <c r="B29" s="38"/>
       <c r="C29" s="20"/>
@@ -2525,156 +2553,80 @@
       <c r="I29" s="50"/>
       <c r="J29" s="20"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="21"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="20"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="21"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="20"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="21"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="20"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="21"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="20"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="21"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="49"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="20"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="20"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="20"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F4 G4 H12:H36 H3:H6 F12:F35 F7:F8">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+  <conditionalFormatting sqref="F2:F4 G4 H3:H6 F7:F9 H13:H29 F13:F28">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F36">
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+  <conditionalFormatting sqref="F29">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2682,7 +2634,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
+  <conditionalFormatting sqref="H8">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2690,7 +2642,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
+  <conditionalFormatting sqref="H9">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>

</xml_diff>

<commit_message>
complete re-work of how shapes are constructed and described.
</commit_message>
<xml_diff>
--- a/SHACL/CJ16050Constraints/TestCases.xlsx
+++ b/SHACL/CJ16050Constraints/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\SENDConform\SHACL\CJ16050Constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F18865-B2CF-46CE-A55C-85BE60BDF254}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC505BC7-7430-4760-871F-9DE0ECDFDEAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5775" activeTab="2" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5780" activeTab="2" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="162">
   <si>
     <t>SD1002</t>
   </si>
@@ -458,32 +458,6 @@
     <t>99T1</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Duplicate USUBJID (test cases only tests </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">within </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>trial)</t>
-    </r>
-  </si>
-  <si>
     <t>99T2</t>
   </si>
   <si>
@@ -496,9 +470,6 @@
     <t>99T2 used to create 2 values for 99T3</t>
   </si>
   <si>
-    <t>99TXXXX used to create two non-unique USUBIJD values for 99TXXXX</t>
-  </si>
-  <si>
     <t>Test Case Data Detail</t>
   </si>
   <si>
@@ -515,9 +486,6 @@
   </si>
   <si>
     <t>TBD</t>
-  </si>
-  <si>
-    <t>UNABLE TO DETERMINE WHEN SUBJID used to create IRIs!</t>
   </si>
   <si>
     <r>
@@ -626,16 +594,7 @@
     <t>No Interval IRI (and not start and end dates)</t>
   </si>
   <si>
-    <t>DateFmtShape</t>
-  </si>
-  <si>
     <t xml:space="preserve">it is possible for an interval to be present but lacking dates. </t>
-  </si>
-  <si>
-    <t>SD1002RuleShape</t>
-  </si>
-  <si>
-    <t>RefIntervalDateShape</t>
   </si>
   <si>
     <t>Interval has missing rfendtc (start with no end)</t>
@@ -671,10 +630,190 @@
     <t>The SD1002 Rule itself: Start Date on or before End Date</t>
   </si>
   <si>
-    <t>SubjectOneRefIntervalShape</t>
-  </si>
-  <si>
     <t>Rules under development</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">One Animal Subject has two </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>subjid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">One Animal Subject has two </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>usubjid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Two Animal Subjects assigned to same </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>subjid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (99T2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Two Animal Subjects assigned to same </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>usubjid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (CJ16050-99T2)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">99T11 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Animal Subject has missing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sujbid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Animal Subject has missing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>usujbid</t>
+    </r>
+  </si>
+  <si>
+    <t>99T12</t>
+  </si>
+  <si>
+    <t>Focus Node</t>
+  </si>
+  <si>
+    <t>Animal_6204e90c</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>hasMin1Max1Shape-SubjID</t>
+  </si>
+  <si>
+    <t>hasMin1Max1Shape-USubjID</t>
+  </si>
+  <si>
+    <t>Animal_252450f2, Animal_2706cb1e</t>
+  </si>
+  <si>
+    <t>Animal_22218ae1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Two Animal Subjects have the same </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>subjid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Two Animal Subjects have the same u</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>subjid</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -684,7 +823,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,14 +885,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -895,7 +1026,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -966,20 +1097,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1008,9 +1135,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1045,13 +1169,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="1" xr:uid="{B3B9F93B-6BDF-408F-A1F2-4D90ACF3B2E0}"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1542,44 +1723,44 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -1594,21 +1775,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B000AF4-3217-4B69-866D-C06BDBC2A333}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="36.5703125" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.1796875" customWidth="1"/>
+    <col min="4" max="4" width="36.54296875" customWidth="1"/>
+    <col min="5" max="5" width="35.54296875" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>74</v>
       </c>
@@ -1628,7 +1809,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="91" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>43</v>
       </c>
@@ -1648,7 +1829,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="104" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
@@ -1668,7 +1849,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="91" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -1688,12 +1869,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>61</v>
@@ -1705,12 +1886,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>29</v>
@@ -1722,7 +1903,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="65" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -1737,7 +1918,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="65" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -1752,7 +1933,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A9" s="28" t="s">
         <v>56</v>
       </c>
@@ -1763,11 +1944,11 @@
       <c r="D9" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="30" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="52" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1784,25 +1965,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A11" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34" t="s">
+      <c r="B11" s="31"/>
+      <c r="C11" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="36" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="F11" s="34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="65" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1817,7 +1998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1832,7 +2013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="52" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1847,7 +2028,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="65" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1862,7 +2043,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>52</v>
       </c>
@@ -1877,7 +2058,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1892,7 +2073,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1907,7 +2088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>71</v>
       </c>
@@ -1922,7 +2103,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>67</v>
       </c>
@@ -1937,7 +2118,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
@@ -1952,7 +2133,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -1982,31 +2163,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F07C322-D3AE-4F2B-B5AA-83448FAE9597}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" style="39" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="39" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" style="37" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="22.1796875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="42.453125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="17" customWidth="1"/>
+    <col min="8" max="8" width="20.453125" customWidth="1"/>
+    <col min="9" max="9" width="6.54296875" style="37" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" style="37" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.26953125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="39" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="37" t="s">
-        <v>145</v>
+      <c r="B1" s="35" t="s">
+        <v>139</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>100</v>
@@ -2015,578 +2198,804 @@
         <v>96</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="I1" s="48" t="s">
-        <v>132</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="I1" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="36">
         <v>1</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>126</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="E2" s="20"/>
       <c r="F2" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="H2" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="I2" s="50">
-        <v>43678</v>
-      </c>
-      <c r="J2" s="20"/>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="21"/>
-      <c r="B3" s="38">
+      <c r="B3" s="36">
         <v>1</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>131</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="E3" s="20"/>
       <c r="F3" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="I3" s="50">
-        <v>43678</v>
-      </c>
-      <c r="J3" s="20"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="20"/>
+    </row>
+    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="42">
         <v>3</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>140</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>119</v>
+        <v>105</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="41" t="s">
+        <v>134</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="H4" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="I4" s="50">
-        <v>43681</v>
-      </c>
-      <c r="J4" s="20"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="20"/>
+    </row>
+    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="42">
         <v>3</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" s="47" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>119</v>
+      <c r="D5" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="63"/>
+      <c r="F5" s="17" t="s">
+        <v>135</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="H5" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="I5" s="50">
-        <v>43681</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="H5" s="20"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="47"/>
+    </row>
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="49">
         <v>3</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>142</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>119</v>
+        <v>141</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41" t="s">
+        <v>136</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="I6" s="50">
-        <v>43681</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="38">
+      <c r="B7" s="36">
         <v>3</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>143</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="E7" s="20"/>
       <c r="F7" s="20" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="H7" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" s="50">
-        <v>43681</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="37">
         <v>2</v>
       </c>
-      <c r="C8" s="53" t="s">
-        <v>148</v>
-      </c>
-      <c r="D8" s="54" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>135</v>
-      </c>
+      <c r="C8" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="51"/>
       <c r="F8" s="20" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="H8" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="I8" s="50">
-        <v>43681</v>
-      </c>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="H8" s="20"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="38">
+      <c r="B9" s="36">
         <v>4</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="G9" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="43"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="53"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" s="56"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="55"/>
+    </row>
+    <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="53"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="55"/>
+      <c r="F12" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" s="56"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="55"/>
+    </row>
+    <row r="13" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="53"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" s="63" t="s">
+        <v>156</v>
+      </c>
+      <c r="I13" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="J13" s="58">
+        <v>43691</v>
+      </c>
+      <c r="K13" s="55"/>
+    </row>
+    <row r="14" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="53"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="I14" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="J14" s="58">
+        <v>43691</v>
+      </c>
+      <c r="K14" s="55"/>
+    </row>
+    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="53"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="F15" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="63" t="s">
+        <v>156</v>
+      </c>
+      <c r="I15" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="J15" s="58">
+        <v>43691</v>
+      </c>
+      <c r="K15" s="55"/>
+    </row>
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="53"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="I16" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="J16" s="58">
+        <v>43691</v>
+      </c>
+      <c r="K16" s="55"/>
+    </row>
+    <row r="17" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="36"/>
+      <c r="C17" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" s="62" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="59"/>
+      <c r="C18" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="48"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="50"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="53"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="55"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="53"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="55"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="53"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="55"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="53"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="55"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="53"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="55"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="53"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="55"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="26" x14ac:dyDescent="0.35">
+      <c r="A28" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="39"/>
+      <c r="C28" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="24"/>
+      <c r="F28" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H28" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I28" s="46"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="20"/>
+    </row>
+    <row r="29" spans="1:11" ht="26" x14ac:dyDescent="0.35">
+      <c r="A29" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="39"/>
+      <c r="C29" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="23"/>
+      <c r="F29" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I29" s="46"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="20"/>
+    </row>
+    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="40"/>
+      <c r="C31" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H31" s="21"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="20"/>
+    </row>
+    <row r="32" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="21"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="G9" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="H9" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="I9" s="50">
-        <v>43681</v>
-      </c>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="55" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="H15" s="49"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="H16" s="49"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="20" t="s">
+      <c r="G32" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="20"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="20"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="20"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="20"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="20"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="20"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="20"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="20"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="20"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="20"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="20"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" s="21"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="20"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" s="21"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="20"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" s="21"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="20"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" s="21"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="20"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37" s="21"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="20"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A38" s="21"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="20"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" s="21"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="20"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40" s="21"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="47"/>
+      <c r="K40" s="20"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41" s="21"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="20"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A42" s="21"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="20"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F4 G4 H3:H6 F7:F9 H13:H29 F13:F28">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+  <conditionalFormatting sqref="G2:G4 H4 I3:I6 I31:I42 G31:G41 H13:H14 I28:I29 I10:I24 G28:G29 G7:G24">
+    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29">
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+  <conditionalFormatting sqref="G42">
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+  <conditionalFormatting sqref="I2">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
     <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2594,7 +3003,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
+  <conditionalFormatting sqref="H7">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2602,7 +3011,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
+  <conditionalFormatting sqref="I7">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2610,7 +3019,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
+  <conditionalFormatting sqref="H8">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2618,7 +3027,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="I8">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2626,7 +3035,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
+  <conditionalFormatting sqref="I9">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2634,7 +3043,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
+  <conditionalFormatting sqref="H15">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2642,7 +3051,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
+  <conditionalFormatting sqref="H16">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>

</xml_diff>

<commit_message>
minor updates, test push to master
</commit_message>
<xml_diff>
--- a/SHACL/CJ16050Constraints/TestCases.xlsx
+++ b/SHACL/CJ16050Constraints/TestCases.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\SENDConform\SHACL\CJ16050Constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC505BC7-7430-4760-871F-9DE0ECDFDEAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A84B2686-C22D-4B1A-B895-5C8A235BC8BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5780" activeTab="2" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5780" activeTab="1" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
     <sheet name="RuleDescriptions" sheetId="1" r:id="rId2"/>
     <sheet name="TestCases" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet1!$A$1:$H$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="182">
   <si>
     <t>SD1002</t>
   </si>
@@ -815,6 +819,68 @@
       <t>subjid</t>
     </r>
   </si>
+  <si>
+    <t>Animal_252450f2</t>
+  </si>
+  <si>
+    <t>99DUP1</t>
+  </si>
+  <si>
+    <t>Animal_2706cb1e</t>
+  </si>
+  <si>
+    <t>SUBJID</t>
+  </si>
+  <si>
+    <t>MISSING</t>
+  </si>
+  <si>
+    <t>99T11/99T11B</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Violation</t>
+  </si>
+  <si>
+    <t>USUBJID</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Test
+Working?</t>
+  </si>
+  <si>
+    <t>IRI</t>
+  </si>
+  <si>
+    <t>ID assigned to more than one Animal</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>Status
+Date</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>ID assigned to more than one Animal:  Animal_252450f2,  Animal_2706cb1e</t>
+  </si>
+  <si>
+    <t>UniqueSubjectIdentifier_CJ16050_99DUP1</t>
+  </si>
 </sst>
 </file>
 
@@ -823,7 +889,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -915,6 +981,28 @@
       <b/>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1026,7 +1114,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1199,12 +1287,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="1" xr:uid="{B3B9F93B-6BDF-408F-A1F2-4D90ACF3B2E0}"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1775,7 +1900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B000AF4-3217-4B69-866D-C06BDBC2A333}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1948,7 +2073,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="52" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -2028,7 +2153,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="65" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -2165,9 +2290,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F07C322-D3AE-4F2B-B5AA-83448FAE9597}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2948,118 +3073,378 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G4 H4 I3:I6 I31:I42 G31:G41 H13:H14 I28:I29 I10:I24 G28:G29 G7:G24">
-    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42">
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CBDD40-5515-4AE9-8EBC-FAD5FA2A6D5D}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.36328125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6328125" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="66" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="67" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" s="20"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="69" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" s="47"/>
+      <c r="H5" s="20"/>
+    </row>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="64" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="20"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" s="47"/>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="68"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="47"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="68"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="20"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="68"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="68"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="68"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="68"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="20"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H8" xr:uid="{2FBF1AF1-330E-470A-82D6-415FA93E716C}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="USUBJID"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="F2:F14">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates to test cases doc
</commit_message>
<xml_diff>
--- a/SHACL/CJ16050Constraints/TestCases.xlsx
+++ b/SHACL/CJ16050Constraints/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\SENDConform\SHACL\CJ16050Constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB45DDFF-1039-4F7D-BEEB-A840647091B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB229807-D77F-48B6-AC97-E6AB4BBC769D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5780" activeTab="1" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5780" activeTab="2" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -2088,7 +2088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B000AF4-3217-4B69-866D-C06BDBC2A333}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
@@ -2509,9 +2509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F07C322-D3AE-4F2B-B5AA-83448FAE9597}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3139,7 +3139,7 @@
       <c r="G17" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="61" t="s">
         <v>114</v>
       </c>
       <c r="I17" s="17"/>
@@ -3162,7 +3162,7 @@
       <c r="G18" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="61" t="s">
         <v>115</v>
       </c>
       <c r="I18" s="17"/>
@@ -3179,7 +3179,7 @@
       <c r="E19" s="48"/>
       <c r="F19" s="48"/>
       <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
+      <c r="H19" s="61"/>
       <c r="I19" s="49"/>
       <c r="J19" s="49"/>
       <c r="K19" s="50"/>
@@ -3190,6 +3190,13 @@
       <c r="A20" s="45" t="s">
         <v>201</v>
       </c>
+      <c r="H20" s="61"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H21" s="61"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H22" s="61"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
@@ -3207,7 +3214,7 @@
       <c r="G23" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H23" s="61" t="s">
         <v>114</v>
       </c>
       <c r="I23" s="23" t="s">
@@ -3234,7 +3241,7 @@
       <c r="G24" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="61" t="s">
         <v>114</v>
       </c>
       <c r="I24" s="23" t="s">
@@ -3396,7 +3403,7 @@
       <c r="M36" s="16"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I12:I13 K10 K23:K24 H23:H24 K27:K36 K12:K19 H27:H35 H15:H19">
+  <conditionalFormatting sqref="I12:I13 K10 K23:K24 K27:K36 K12:K19 H27:H35 H15">
     <cfRule type="cellIs" dxfId="33" priority="57" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>

</xml_diff>

<commit_message>
test update of pages
</commit_message>
<xml_diff>
--- a/SHACL/CJ16050Constraints/TestCases.xlsx
+++ b/SHACL/CJ16050Constraints/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\SENDConform\SHACL\CJ16050Constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB229807-D77F-48B6-AC97-E6AB4BBC769D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0A25E9-6035-42EA-B8DC-87B589F55340}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5780" activeTab="2" xr2:uid="{5508F746-7D09-453C-97D0-4584F496F062}"/>
   </bookViews>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet1!$A$1:$H$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$1:$M$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="197">
   <si>
     <t>SD1002</t>
   </si>
@@ -491,15 +492,6 @@
     <t>99T1</t>
   </si>
   <si>
-    <t>99T2</t>
-  </si>
-  <si>
-    <t>99T5</t>
-  </si>
-  <si>
-    <t>99T4</t>
-  </si>
-  <si>
     <t>99T2 used to create 2 values for 99T3</t>
   </si>
   <si>
@@ -589,25 +581,10 @@
     <t>Link our data to teh SEND ontology</t>
   </si>
   <si>
-    <t>99T2 (99T2,99T3)</t>
-  </si>
-  <si>
-    <t>99T6,99T7</t>
-  </si>
-  <si>
     <t>rfendtc as xsd:string  "7-Dec-2016"</t>
   </si>
   <si>
     <t>One RFSTDTC/RFENDTC per AnimalSubject</t>
-  </si>
-  <si>
-    <t>99T8</t>
-  </si>
-  <si>
-    <t>99T9</t>
-  </si>
-  <si>
-    <t>99T10</t>
   </si>
   <si>
     <t>rfstdtc as xsd:string  "6-DEC-2016"</t>
@@ -637,11 +614,6 @@
   </si>
   <si>
     <t xml:space="preserve">Interval with &gt;1 rfstdtc and &gt;1 rfendtc </t>
-  </si>
-  <si>
-    <t>99T11
-99T2
-99T</t>
   </si>
   <si>
     <t>Rule
@@ -677,9 +649,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">99T11 </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Animal Subject has missing </t>
     </r>
@@ -714,9 +683,6 @@
     </r>
   </si>
   <si>
-    <t>99T12</t>
-  </si>
-  <si>
     <t>Focus Node</t>
   </si>
   <si>
@@ -730,9 +696,6 @@
   </si>
   <si>
     <t>hasMin1Max1Shape-USubjID</t>
-  </si>
-  <si>
-    <t>Animal_252450f2, Animal_2706cb1e</t>
   </si>
   <si>
     <t>Animal_22218ae1</t>
@@ -798,27 +761,6 @@
   </si>
   <si>
     <t>UniqueSubjectIdentifier_CJ16050_99DUP1</t>
-  </si>
-  <si>
-    <t>Animal_68bab561</t>
-  </si>
-  <si>
-    <t>Animal_56cbc8c2</t>
-  </si>
-  <si>
-    <t>Animal_db3c6403</t>
-  </si>
-  <si>
-    <t>Animal_6f395f06</t>
-  </si>
-  <si>
-    <t>Animal_24908fa7</t>
-  </si>
-  <si>
-    <t>Animal_21316392</t>
-  </si>
-  <si>
-    <t>Animal_184f16eb</t>
   </si>
   <si>
     <t>isUniqueShape-USubjID</t>
@@ -929,14 +871,6 @@
     </r>
   </si>
   <si>
-    <t>Animal_21316392
-(Animal_21316392, T3)</t>
-  </si>
-  <si>
-    <t>Animal_6204e90c(T11)
-Animal_21316392</t>
-  </si>
-  <si>
     <t>hasTypeXsdDateShape-Date</t>
   </si>
   <si>
@@ -996,6 +930,57 @@
   </si>
   <si>
     <t>BRTHDTC not present in test data</t>
+  </si>
+  <si>
+    <t>Animal_xxxxxxx</t>
+  </si>
+  <si>
+    <t>Animal_5dba5b4b, Animal_1a2751f1</t>
+  </si>
+  <si>
+    <t>Animal_69fa85ac</t>
+  </si>
+  <si>
+    <t>99T3</t>
+  </si>
+  <si>
+    <t>An Animal Subject cannot have more than one USUBJID.</t>
+  </si>
+  <si>
+    <t>Animal_2a836191</t>
+  </si>
+  <si>
+    <t>99T1, 99T2</t>
+  </si>
+  <si>
+    <t>99T4,99T5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Animal subject has two </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>usubjid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> values</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1270,7 +1255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1408,9 +1393,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2188,7 +2170,7 @@
         <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>60</v>
@@ -2206,7 +2188,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>28</v>
@@ -2251,18 +2233,18 @@
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" s="78" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A9" s="75" t="s">
+    <row r="9" spans="1:6" s="77" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A9" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="76" t="s">
+      <c r="B9" s="74"/>
+      <c r="C9" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="76" t="s">
+      <c r="D9" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="77" t="s">
+      <c r="E9" s="76" t="s">
         <v>58</v>
       </c>
       <c r="F9" s="36"/>
@@ -2299,8 +2281,8 @@
       <c r="E11" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="60" t="s">
-        <v>118</v>
+      <c r="F11" s="59" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -2314,10 +2296,10 @@
         <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="F12" s="17"/>
     </row>
@@ -2330,7 +2312,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>5</v>
@@ -2386,43 +2368,43 @@
       <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="71" t="s">
+      <c r="C17" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="71" t="s">
+      <c r="D17" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="72" t="s">
+      <c r="E17" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="73" t="s">
-        <v>206</v>
+      <c r="F17" s="72" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="73" t="s">
-        <v>207</v>
+      <c r="F18" s="72" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -2458,42 +2440,42 @@
       <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="70" t="s">
+      <c r="C21" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="70" t="s">
+      <c r="D21" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="70" t="s">
+      <c r="E21" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="70" t="s">
-        <v>208</v>
+      <c r="F21" s="69" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="70" t="s">
+      <c r="B22" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="70" t="s">
+      <c r="C22" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="70" t="s">
+      <c r="D22" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="70" t="s">
+      <c r="E22" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="70" t="s">
+      <c r="F22" s="69" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2507,11 +2489,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F07C322-D3AE-4F2B-B5AA-83448FAE9597}">
-  <dimension ref="A1:M36"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2535,43 +2518,43 @@
         <v>73</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>99</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>95</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>97</v>
       </c>
       <c r="J1" s="38" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="K1" s="38" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="L1" s="38" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
@@ -2579,75 +2562,71 @@
         <v>1</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="K2" s="39" t="s">
         <v>137</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="H2" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="K2" s="39" t="s">
-        <v>148</v>
       </c>
       <c r="L2" s="40">
         <v>43691</v>
       </c>
       <c r="M2" s="16"/>
     </row>
-    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17"/>
       <c r="B3" s="29">
         <v>1</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="K3" s="39" t="s">
         <v>137</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="H3" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="K3" s="39" t="s">
-        <v>148</v>
       </c>
       <c r="L3" s="40">
         <v>43691</v>
       </c>
       <c r="M3" s="16"/>
     </row>
-    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
@@ -2655,38 +2634,36 @@
         <v>3</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>103</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="E4" s="16"/>
       <c r="F4" s="16" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="H4" s="61" t="s">
-        <v>114</v>
+        <v>123</v>
+      </c>
+      <c r="H4" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="K4" s="39" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="L4" s="40">
         <v>43691</v>
       </c>
       <c r="M4" s="16"/>
     </row>
-    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>0</v>
       </c>
@@ -2694,37 +2671,35 @@
         <v>3</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="62" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="G5" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="F5" s="52" t="s">
-        <v>176</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H5" s="61" t="s">
-        <v>114</v>
+      <c r="H5" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="K5" s="39" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="L5" s="40">
         <v>43691</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>0</v>
       </c>
@@ -2732,40 +2707,38 @@
         <v>3</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="F6" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="34"/>
+      <c r="F6" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="I6" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="G6" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H6" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>198</v>
-      </c>
       <c r="J6" s="17" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="K6" s="39" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="L6" s="40">
         <v>43691</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
@@ -2773,40 +2746,36 @@
         <v>3</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>195</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
       <c r="G7" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="H7" s="61" t="s">
-        <v>114</v>
+        <v>126</v>
+      </c>
+      <c r="H7" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="K7" s="39" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="L7" s="40">
         <v>43691</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="41" t="s">
         <v>0</v>
       </c>
@@ -2814,38 +2783,34 @@
         <v>2</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>196</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="E8" s="44"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="H8" s="61" t="s">
-        <v>114</v>
+        <v>171</v>
+      </c>
+      <c r="H8" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="K8" s="39" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="L8" s="40">
         <v>43691</v>
       </c>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>0</v>
       </c>
@@ -2853,31 +2818,31 @@
         <v>4</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>101</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="61" t="s">
-        <v>114</v>
+      <c r="H9" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="K9" s="39" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="L9" s="40">
         <v>43691</v>
@@ -2892,38 +2857,32 @@
         <v>3</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>102</v>
+        <v>195</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="H10" s="61" t="s">
-        <v>114</v>
+        <v>175</v>
+      </c>
+      <c r="H10" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I10" s="43" t="s">
-        <v>180</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="K10" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="L10" s="40">
-        <v>43691</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="J10" s="17"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>55</v>
       </c>
@@ -2931,38 +2890,34 @@
         <v>3</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>151</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="H11" s="61" t="s">
-        <v>114</v>
+        <v>174</v>
+      </c>
+      <c r="H11" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I11" s="43" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="L11" s="40">
         <v>43691</v>
       </c>
       <c r="M11" s="16"/>
     </row>
-    <row r="12" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>55</v>
       </c>
@@ -2970,31 +2925,29 @@
         <v>1</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>142</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="E12" s="16"/>
       <c r="F12" s="16" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="H12" s="61" t="s">
-        <v>114</v>
+        <v>132</v>
+      </c>
+      <c r="H12" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I12" s="43" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="K12" s="39" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="L12" s="40">
         <v>43691</v>
@@ -3009,138 +2962,132 @@
         <v>2</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="D13" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>145</v>
-      </c>
       <c r="F13" s="16" t="s">
-        <v>152</v>
+        <v>190</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="H13" s="61" t="s">
-        <v>114</v>
+        <v>134</v>
+      </c>
+      <c r="H13" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I13" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="K13" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="L13" s="40">
-        <v>43691</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="J13" s="17"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="40"/>
       <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="31">
+        <v>1</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="H14" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14" s="43"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B15" s="29">
         <v>2</v>
       </c>
-      <c r="C14" s="41" t="s">
-        <v>185</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>192</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="H14" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="I14" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="K14" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="L14" s="40">
+      <c r="C15" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="K15" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="L15" s="40">
         <v>43691</v>
       </c>
-      <c r="M14" s="16"/>
-    </row>
-    <row r="15" spans="1:13" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="63"/>
-      <c r="B15" s="64"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="65"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" s="68" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="62"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="64"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="H16" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="16"/>
-    </row>
-    <row r="17" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="33"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="16" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D17" s="16"/>
-      <c r="E17" s="16" t="s">
-        <v>102</v>
-      </c>
+      <c r="E17" s="16"/>
       <c r="F17" s="16" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="H17" s="61" t="s">
-        <v>114</v>
+        <v>107</v>
+      </c>
+      <c r="H17" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
@@ -3149,21 +3096,23 @@
       <c r="M17" s="16"/>
     </row>
     <row r="18" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="17"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="33"/>
       <c r="C18" s="16" t="s">
         <v>113</v>
       </c>
       <c r="D18" s="16"/>
-      <c r="E18" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16" t="s">
+        <v>188</v>
+      </c>
       <c r="G18" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" s="61" t="s">
-        <v>115</v>
+        <v>109</v>
+      </c>
+      <c r="H18" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I18" s="17"/>
       <c r="J18" s="17"/>
@@ -3171,78 +3120,72 @@
       <c r="L18" s="40"/>
       <c r="M18" s="16"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="46"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="48"/>
+    <row r="19" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="17"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="45" t="s">
-        <v>201</v>
-      </c>
-      <c r="H20" s="61"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="48"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H21" s="61"/>
+      <c r="A21" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="H21" s="60"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H22" s="61"/>
+      <c r="H22" s="60"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="H23" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="J23" s="23"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="16"/>
+      <c r="H23" s="60"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="19" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B24" s="32"/>
       <c r="C24" s="21" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D24" s="21"/>
-      <c r="E24" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="H24" s="61" t="s">
-        <v>114</v>
+      <c r="E24" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="20"/>
+      <c r="G24" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="I24" s="23" t="s">
         <v>100</v>
@@ -3252,20 +3195,30 @@
       <c r="L24" s="40"/>
       <c r="M24" s="16"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="17"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="16"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" s="23"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="16"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="17"/>
@@ -3402,8 +3355,30 @@
       <c r="L36" s="40"/>
       <c r="M36" s="16"/>
     </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" s="17"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="16"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="I12:I13 K10 K23:K24 K27:K36 K12:K19 H27:H35 H15">
+  <autoFilter ref="A1:M15" xr:uid="{A1B5E1BC-6AD1-47B6-89FE-ED3EDC07BEB2}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="SD0083"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="I12:I14 K10 K24:K25 K28:K37 K12:K20 H28:H36 H16">
     <cfRule type="cellIs" dxfId="33" priority="57" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -3411,7 +3386,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
+  <conditionalFormatting sqref="H37">
     <cfRule type="cellIs" dxfId="31" priority="55" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -3427,7 +3402,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
+  <conditionalFormatting sqref="K17">
     <cfRule type="cellIs" dxfId="27" priority="19" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -3443,7 +3418,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
+  <conditionalFormatting sqref="I15">
     <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -3451,7 +3426,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
+  <conditionalFormatting sqref="I13:I14">
     <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -3548,7 +3523,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.36328125" style="59" customWidth="1"/>
+    <col min="1" max="1" width="33.36328125" style="58" customWidth="1"/>
     <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.90625" style="13" customWidth="1"/>
     <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
@@ -3556,169 +3531,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>156</v>
+      <c r="A1" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>144</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="D1" s="54" t="s">
-        <v>159</v>
-      </c>
-      <c r="E1" s="54" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="D1" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>148</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
-        <v>172</v>
+      <c r="A2" s="55" t="s">
+        <v>160</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="17" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="40"/>
       <c r="H2" s="16" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="17" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="40"/>
       <c r="H3" s="16" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="40"/>
       <c r="H4" s="16" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="58" t="s">
-        <v>147</v>
+      <c r="A5" s="57" t="s">
+        <v>136</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="G5" s="40"/>
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
-        <v>147</v>
+      <c r="A6" s="52" t="s">
+        <v>136</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>168</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="40"/>
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="57" t="s">
-        <v>152</v>
+      <c r="A7" s="56" t="s">
+        <v>140</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="17" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="G7" s="40"/>
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="17" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="40"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="57"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="17"/>
       <c r="C9" s="16"/>
       <c r="D9" s="17"/>
@@ -3727,7 +3702,7 @@
       <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="57"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="17"/>
       <c r="C10" s="16"/>
       <c r="D10" s="17"/>
@@ -3737,7 +3712,7 @@
       <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="57"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="17"/>
       <c r="C11" s="16"/>
       <c r="D11" s="17"/>
@@ -3747,7 +3722,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="57"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="17"/>
       <c r="C12" s="16"/>
       <c r="D12" s="17"/>
@@ -3757,7 +3732,7 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="57"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="17"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
@@ -3767,7 +3742,7 @@
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="57"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="17"/>
       <c r="C14" s="16"/>
       <c r="D14" s="17"/>

</xml_diff>